<commit_message>
Phân loại các file overview
</commit_message>
<xml_diff>
--- a/Knowledge/00.Template/nn_ObjName_Overview_date.xlsx
+++ b/Knowledge/00.Template/nn_ObjName_Overview_date.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AndroidKnowledge\00.Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SpringBootPrj\Knowledge\00.Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BE95FE-E851-4E68-8B2B-329DF1B61464}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DC1A59-3FDA-4F14-81E3-EECA6CA801DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>2020/01/07</t>
     <phoneticPr fontId="5"/>
@@ -467,6 +467,41 @@
         <charset val="128"/>
       </rPr>
       <t>ợng&gt;</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Chức năng 1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Chức năng 1.1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <r>
+      <t>Mô tả chức năng
+**Các điểm cần l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Meiryo UI"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>u ý:</t>
     </r>
     <phoneticPr fontId="3"/>
   </si>
@@ -1205,6 +1240,75 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1237,75 +1341,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1775,10 +1810,10 @@
       <c r="B2" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="78"/>
+      <c r="D2" s="101"/>
       <c r="E2" s="36"/>
       <c r="F2" s="37"/>
     </row>
@@ -1789,8 +1824,8 @@
       <c r="B3" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="77"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="100"/>
       <c r="E3" s="36"/>
       <c r="F3" s="37"/>
     </row>
@@ -1801,10 +1836,10 @@
       <c r="B4" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="100"/>
       <c r="E4" s="36"/>
       <c r="F4" s="37"/>
     </row>
@@ -1815,8 +1850,8 @@
       <c r="B5" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
       <c r="E5" s="36"/>
       <c r="F5" s="42"/>
     </row>
@@ -1827,16 +1862,16 @@
       <c r="B6" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
       <c r="E6" s="36"/>
       <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="73">
+      <c r="A7" s="96">
         <v>6</v>
       </c>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="103" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="44" t="s">
@@ -1849,34 +1884,34 @@
       <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="74"/>
-      <c r="B8" s="81"/>
+      <c r="A8" s="97"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="46"/>
       <c r="D8" s="47"/>
       <c r="E8" s="36"/>
       <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="74"/>
-      <c r="B9" s="81"/>
+      <c r="A9" s="97"/>
+      <c r="B9" s="104"/>
       <c r="C9" s="46"/>
       <c r="D9" s="47"/>
       <c r="E9" s="36"/>
       <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="75"/>
-      <c r="B10" s="82"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="46"/>
       <c r="D10" s="47"/>
       <c r="E10" s="36"/>
       <c r="F10" s="37"/>
     </row>
     <row r="11" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="73">
+      <c r="A11" s="96">
         <v>7</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="103" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -1889,42 +1924,42 @@
       <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="74"/>
-      <c r="B12" s="81"/>
+      <c r="A12" s="97"/>
+      <c r="B12" s="104"/>
       <c r="C12" s="48"/>
       <c r="D12" s="47"/>
       <c r="E12" s="36"/>
       <c r="F12" s="37"/>
     </row>
     <row r="13" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="74"/>
-      <c r="B13" s="81"/>
+      <c r="A13" s="97"/>
+      <c r="B13" s="104"/>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
       <c r="E13" s="36"/>
       <c r="F13" s="37"/>
     </row>
     <row r="14" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="74"/>
-      <c r="B14" s="81"/>
+      <c r="A14" s="97"/>
+      <c r="B14" s="104"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
       <c r="E14" s="36"/>
       <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="75"/>
-      <c r="B15" s="82"/>
+      <c r="A15" s="98"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="49"/>
       <c r="D15" s="49"/>
       <c r="E15" s="36"/>
       <c r="F15" s="37"/>
     </row>
     <row r="16" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="73">
+      <c r="A16" s="96">
         <v>8</v>
       </c>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="103" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="44" t="s">
@@ -1937,42 +1972,42 @@
       <c r="F16" s="37"/>
     </row>
     <row r="17" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="74"/>
-      <c r="B17" s="81"/>
+      <c r="A17" s="97"/>
+      <c r="B17" s="104"/>
       <c r="C17" s="48"/>
       <c r="D17" s="47"/>
       <c r="E17" s="36"/>
       <c r="F17" s="37"/>
     </row>
     <row r="18" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="74"/>
-      <c r="B18" s="81"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="104"/>
       <c r="C18" s="49"/>
       <c r="D18" s="49"/>
       <c r="E18" s="36"/>
       <c r="F18" s="37"/>
     </row>
     <row r="19" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="74"/>
-      <c r="B19" s="81"/>
+      <c r="A19" s="97"/>
+      <c r="B19" s="104"/>
       <c r="C19" s="49"/>
       <c r="D19" s="49"/>
       <c r="E19" s="36"/>
       <c r="F19" s="37"/>
     </row>
     <row r="20" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="75"/>
-      <c r="B20" s="82"/>
+      <c r="A20" s="98"/>
+      <c r="B20" s="105"/>
       <c r="C20" s="49"/>
       <c r="D20" s="49"/>
       <c r="E20" s="36"/>
       <c r="F20" s="37"/>
     </row>
     <row r="21" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="73">
+      <c r="A21" s="96">
         <v>8</v>
       </c>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="103" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="44" t="s">
@@ -1985,42 +2020,42 @@
       <c r="F21" s="37"/>
     </row>
     <row r="22" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="74"/>
-      <c r="B22" s="81"/>
+      <c r="A22" s="97"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="48"/>
       <c r="D22" s="47"/>
       <c r="E22" s="36"/>
       <c r="F22" s="37"/>
     </row>
     <row r="23" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="74"/>
-      <c r="B23" s="81"/>
+      <c r="A23" s="97"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="49"/>
       <c r="D23" s="49"/>
       <c r="E23" s="36"/>
       <c r="F23" s="37"/>
     </row>
     <row r="24" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="74"/>
-      <c r="B24" s="81"/>
+      <c r="A24" s="97"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="49"/>
       <c r="D24" s="49"/>
       <c r="E24" s="36"/>
       <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="75"/>
-      <c r="B25" s="82"/>
+      <c r="A25" s="98"/>
+      <c r="B25" s="105"/>
       <c r="C25" s="49"/>
       <c r="D25" s="49"/>
       <c r="E25" s="36"/>
       <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="73">
+      <c r="A26" s="96">
         <v>8</v>
       </c>
-      <c r="B26" s="80" t="s">
+      <c r="B26" s="103" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="44" t="s">
@@ -2033,32 +2068,32 @@
       <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:6" s="30" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="74"/>
-      <c r="B27" s="81"/>
+      <c r="A27" s="97"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="48"/>
       <c r="D27" s="47"/>
       <c r="E27" s="36"/>
       <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="74"/>
-      <c r="B28" s="81"/>
+      <c r="A28" s="97"/>
+      <c r="B28" s="104"/>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
       <c r="E28" s="36"/>
       <c r="F28" s="37"/>
     </row>
     <row r="29" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="74"/>
-      <c r="B29" s="81"/>
+      <c r="A29" s="97"/>
+      <c r="B29" s="104"/>
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
       <c r="E29" s="36"/>
       <c r="F29" s="37"/>
     </row>
     <row r="30" spans="1:6" s="30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="75"/>
-      <c r="B30" s="82"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="105"/>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
       <c r="E30" s="36"/>
@@ -2071,8 +2106,8 @@
       <c r="B31" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="77"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="100"/>
       <c r="E31" s="36"/>
       <c r="F31" s="37"/>
     </row>
@@ -2083,8 +2118,8 @@
       <c r="B32" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="79"/>
-      <c r="D32" s="77"/>
+      <c r="C32" s="102"/>
+      <c r="D32" s="100"/>
       <c r="E32" s="36"/>
       <c r="F32" s="37"/>
     </row>
@@ -2241,126 +2276,134 @@
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="74" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="48" x14ac:dyDescent="0.4">
-      <c r="B4" s="86">
+      <c r="B4" s="75">
         <f>ROW()-3</f>
         <v>1</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="88" t="s">
+      <c r="E4" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="89"/>
-      <c r="G4" s="90" t="s">
+      <c r="F4" s="78"/>
+      <c r="G4" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="91"/>
+      <c r="H4" s="80"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B5" s="86">
+      <c r="B5" s="75">
         <f t="shared" ref="B5:B9" si="0">ROW()-3</f>
         <v>2</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="88" t="s">
+      <c r="E5" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="89"/>
-      <c r="G5" s="87" t="s">
+      <c r="F5" s="78"/>
+      <c r="G5" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="91"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B6" s="86">
+      <c r="H5" s="80"/>
+    </row>
+    <row r="6" spans="2:8" ht="36" x14ac:dyDescent="0.4">
+      <c r="B6" s="75">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="91"/>
+      <c r="C6" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="78"/>
+      <c r="G6" s="76" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="80"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B7" s="86">
+      <c r="B7" s="75">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="91"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="80"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="86">
+      <c r="B8" s="75">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="92"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="87"/>
-      <c r="H8" s="91"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="80"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="86">
+      <c r="B9" s="75">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="92"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="91"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="80"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="96"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="85"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
@@ -2429,51 +2472,51 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="59"/>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="98" t="s">
+      <c r="F3" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="97" t="s">
+      <c r="G3" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="99"/>
+      <c r="J3" s="88"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="59"/>
-      <c r="B4" s="100">
+      <c r="B4" s="89">
         <f>ROW()-3</f>
         <v>1</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="101"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="105" t="str">
+      <c r="D4" s="90"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="94" t="str">
         <f ca="1">HYPERLINK("["&amp;SUBSTITUTE(CELL("filename"),TRIM(RIGHT(SUBSTITUTE(CELL("filename"),"\",REPT(" ",255)),255)),"")&amp;"Samples\No"&amp;B4&amp;".xlsx]","click")</f>
         <v>click</v>
       </c>
-      <c r="J4" s="99"/>
+      <c r="J4" s="88"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>